<commit_message>
Documentation of Randomic Alg
</commit_message>
<xml_diff>
--- a/Guia e Tarefas/Comparativo Aleatorio x Estado da Arte.xlsx
+++ b/Guia e Tarefas/Comparativo Aleatorio x Estado da Arte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Engenharia de Software\GitHub\Maximum-Diversity-Problem\Guia e Tarefas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3600452C-4338-49BC-9D02-9C43059D0DFA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D2A011-BC5D-4D3D-911B-CFCD6FAB5F78}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4590" xr2:uid="{E338D036-04EB-4397-B8B0-CB76D9CD48AC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="15">
   <si>
     <t>Tempo de Execução</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>GKD-c_1_n500_m50.txt</t>
+  </si>
+  <si>
+    <t>GKD-c_1_n500_m50</t>
   </si>
 </sst>
 </file>
@@ -87,15 +90,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -104,18 +113,56 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color indexed="8"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="hair">
-        <color indexed="8"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
-      <top style="hair">
-        <color indexed="8"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="hair">
-        <color indexed="8"/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -125,14 +172,14 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -448,136 +495,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5527C57B-B6B6-40B1-A824-06DAFAB611D7}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="B2:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D2" s="4"/>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D4" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E4" s="8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
+      <c r="C5" s="1">
         <v>285</v>
       </c>
-      <c r="C4">
+      <c r="D5" s="1">
         <v>333</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="E5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="C6" s="1">
         <v>1028</v>
       </c>
-      <c r="C5">
+      <c r="D6" s="1">
         <v>1247</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="E6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
+      <c r="C7" s="1">
         <v>8521</v>
       </c>
-      <c r="C6" s="3">
+      <c r="D7" s="2">
         <v>9689</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
+      <c r="C8" s="1">
         <v>6553</v>
       </c>
-      <c r="C7" s="4">
+      <c r="D8" s="2">
         <v>7833.8325199999999</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
+      <c r="C9" s="1">
         <v>101341</v>
       </c>
-      <c r="C8" s="5">
+      <c r="D9" s="2">
         <v>114259</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E9" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
+      <c r="C10" s="1">
         <v>101333</v>
       </c>
-      <c r="C9" s="6">
+      <c r="D10" s="2">
         <v>114191</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="E10" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="1">
         <v>17199</v>
       </c>
-      <c r="C10" s="8">
+      <c r="D11" s="2">
         <v>19485.1875</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E11" s="2" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>